<commit_message>
Updated table with latest covid2019 received data.
</commit_message>
<xml_diff>
--- a/Data/Covid2019/SA_data_archive/Gauteng/Covid 19 Data.xlsx
+++ b/Data/Covid2019/SA_data_archive/Gauteng/Covid 19 Data.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bonpro-my.sharepoint.com/personal/bongani_bonpro_co_za/Documents/Other/COVID 19 Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="391" documentId="8_{4BD55CDF-CBCA-4C9E-8D86-F86C8560E47A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C52CFD1C-9D16-4A61-AB73-8E6803743D48}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{A7BD6684-BF9F-4A3B-A140-878706D3E08F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="District" sheetId="1" r:id="rId1"/>
-    <sheet name="Regions" sheetId="2" r:id="rId2"/>
+    <sheet name="sub-District" sheetId="2" r:id="rId2"/>
     <sheet name="National" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>District</t>
   </si>
@@ -91,15 +85,6 @@
     <t>Region G</t>
   </si>
   <si>
-    <t>East</t>
-  </si>
-  <si>
-    <t>North</t>
-  </si>
-  <si>
-    <t>South</t>
-  </si>
-  <si>
     <t>Region 1</t>
   </si>
   <si>
@@ -138,12 +123,48 @@
   <si>
     <t>Merafong</t>
   </si>
+  <si>
+    <t>East 1</t>
+  </si>
+  <si>
+    <t>East 2</t>
+  </si>
+  <si>
+    <t>North 1</t>
+  </si>
+  <si>
+    <t>North 2</t>
+  </si>
+  <si>
+    <t>South 1</t>
+  </si>
+  <si>
+    <t>South 2</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>City of Johannesburg - Recoveries</t>
+  </si>
+  <si>
+    <t>Ekurhuleni - Recoveries</t>
+  </si>
+  <si>
+    <t>City of Tshwane - Recoveries</t>
+  </si>
+  <si>
+    <t>Sedibeng - Recoveries</t>
+  </si>
+  <si>
+    <t>Westrand - Recoveries</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,8 +210,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +244,14 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -246,13 +289,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -265,6 +336,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -327,7 +407,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -379,7 +459,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -573,43 +653,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3879E26A-A6F4-4151-939A-E112DD311752}">
-  <dimension ref="A1:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" customWidth="1"/>
+    <col min="13" max="13" width="10.54296875" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
-    <col min="17" max="17" width="9.88671875" customWidth="1"/>
-    <col min="18" max="18" width="9.77734375" customWidth="1"/>
+    <col min="16" max="16" width="9.6328125" customWidth="1"/>
+    <col min="17" max="17" width="9.90625" customWidth="1"/>
+    <col min="18" max="18" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,8 +745,20 @@
       <c r="R1" s="2">
         <v>43952</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" s="2">
+        <v>43953</v>
+      </c>
+      <c r="T1" s="2">
+        <v>43954</v>
+      </c>
+      <c r="U1" s="2">
+        <v>43955</v>
+      </c>
+      <c r="V1" s="2">
+        <v>43956</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -708,8 +801,29 @@
       <c r="N2">
         <v>804</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O2">
+        <v>811</v>
+      </c>
+      <c r="P2">
+        <v>828</v>
+      </c>
+      <c r="Q2">
+        <v>840</v>
+      </c>
+      <c r="R2">
+        <v>865</v>
+      </c>
+      <c r="S2">
+        <v>920</v>
+      </c>
+      <c r="T2">
+        <v>935</v>
+      </c>
+      <c r="U2">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -752,8 +866,29 @@
       <c r="N3">
         <v>300</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O3">
+        <v>310</v>
+      </c>
+      <c r="P3">
+        <v>318</v>
+      </c>
+      <c r="Q3">
+        <v>319</v>
+      </c>
+      <c r="R3">
+        <v>328</v>
+      </c>
+      <c r="S3">
+        <v>349</v>
+      </c>
+      <c r="T3">
+        <v>358</v>
+      </c>
+      <c r="U3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -796,8 +931,29 @@
       <c r="N4">
         <v>136</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O4">
+        <v>144</v>
+      </c>
+      <c r="P4">
+        <v>149</v>
+      </c>
+      <c r="Q4">
+        <v>172</v>
+      </c>
+      <c r="R4">
+        <v>187</v>
+      </c>
+      <c r="S4">
+        <v>201</v>
+      </c>
+      <c r="T4">
+        <v>201</v>
+      </c>
+      <c r="U4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -840,8 +996,29 @@
       <c r="N5">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O5">
+        <v>15</v>
+      </c>
+      <c r="P5">
+        <v>16</v>
+      </c>
+      <c r="Q5">
+        <v>16</v>
+      </c>
+      <c r="R5">
+        <v>18</v>
+      </c>
+      <c r="S5">
+        <v>19</v>
+      </c>
+      <c r="T5">
+        <v>21</v>
+      </c>
+      <c r="U5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -884,8 +1061,29 @@
       <c r="N6">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O6">
+        <v>43</v>
+      </c>
+      <c r="P6">
+        <v>43</v>
+      </c>
+      <c r="Q6">
+        <v>44</v>
+      </c>
+      <c r="R6">
+        <v>45</v>
+      </c>
+      <c r="S6">
+        <v>45</v>
+      </c>
+      <c r="T6">
+        <v>45</v>
+      </c>
+      <c r="U6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -928,8 +1126,29 @@
       <c r="N7">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O7">
+        <v>54</v>
+      </c>
+      <c r="P7">
+        <v>54</v>
+      </c>
+      <c r="Q7">
+        <v>55</v>
+      </c>
+      <c r="R7">
+        <v>64</v>
+      </c>
+      <c r="S7">
+        <v>64</v>
+      </c>
+      <c r="T7">
+        <v>64</v>
+      </c>
+      <c r="U7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -972,12 +1191,30 @@
       <c r="N8" s="3">
         <v>1353</v>
       </c>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O8" s="3">
+        <v>1377</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1408</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1446</v>
+      </c>
+      <c r="R8" s="3">
+        <v>1507</v>
+      </c>
+      <c r="S8" s="3">
+        <v>1598</v>
+      </c>
+      <c r="T8" s="3">
+        <v>1624</v>
+      </c>
+      <c r="U8" s="3">
+        <v>1661</v>
+      </c>
+      <c r="V8" s="3"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1020,12 +1257,30 @@
       <c r="N9" s="3">
         <v>8</v>
       </c>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O9" s="3">
+        <v>8</v>
+      </c>
+      <c r="P9" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>11</v>
+      </c>
+      <c r="R9" s="3">
+        <v>12</v>
+      </c>
+      <c r="S9" s="3">
+        <v>12</v>
+      </c>
+      <c r="T9" s="3">
+        <v>14</v>
+      </c>
+      <c r="U9" s="3">
+        <v>14</v>
+      </c>
+      <c r="V9" s="3"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1068,52 +1323,327 @@
       <c r="N10" s="3">
         <v>876</v>
       </c>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O10" s="3">
+        <v>897</v>
+      </c>
+      <c r="P10" s="3">
+        <v>897</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>948</v>
+      </c>
+      <c r="R10" s="3">
+        <v>948</v>
+      </c>
+      <c r="S10" s="3">
+        <v>979</v>
+      </c>
+      <c r="T10" s="3">
+        <v>1015</v>
+      </c>
+      <c r="U10" s="3">
+        <v>1026</v>
+      </c>
+      <c r="V10" s="3"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="B11" s="3">
+        <f>B8-B9-B10</f>
+        <v>446</v>
+      </c>
+      <c r="C11" s="3">
+        <f>C8-C9-C10</f>
+        <v>484</v>
+      </c>
+      <c r="D11" s="3">
+        <f>D8-D9-D10</f>
+        <v>472</v>
+      </c>
+      <c r="E11" s="3">
+        <f>E8-E9-E10</f>
+        <v>550</v>
+      </c>
+      <c r="F11" s="3">
+        <f>F8-F9-F10</f>
+        <v>591</v>
+      </c>
+      <c r="G11" s="3">
+        <f>G8-G9-G10</f>
+        <v>589</v>
+      </c>
+      <c r="H11" s="3">
+        <f>H8-H9-H10</f>
+        <v>411</v>
+      </c>
+      <c r="I11" s="3">
+        <f>I8-I9-I10</f>
+        <v>391</v>
+      </c>
+      <c r="J11" s="3">
+        <f>J8-J9-J10</f>
+        <v>401</v>
+      </c>
+      <c r="K11" s="3">
+        <f>K8-K9-K10</f>
+        <v>427</v>
+      </c>
+      <c r="L11" s="3">
+        <f>L8-L9-L10</f>
+        <v>441</v>
+      </c>
+      <c r="M11" s="3">
+        <f>M8-M9-M10</f>
+        <v>455</v>
+      </c>
+      <c r="N11" s="3">
+        <f>N8-N9-N10</f>
+        <v>469</v>
+      </c>
+      <c r="O11" s="3">
+        <f>O8-O9-O10</f>
+        <v>472</v>
+      </c>
+      <c r="P11" s="3">
+        <f>P8-P9-P10</f>
+        <v>500</v>
+      </c>
+      <c r="Q11" s="3">
+        <f>Q8-Q9-Q10</f>
+        <v>487</v>
+      </c>
+      <c r="R11" s="3">
+        <f>R8-R9-R10</f>
+        <v>547</v>
+      </c>
+      <c r="S11" s="3">
+        <f>S8-S9-S10</f>
+        <v>607</v>
+      </c>
+      <c r="T11" s="3">
+        <f>T8-T9-T10</f>
+        <v>595</v>
+      </c>
+      <c r="U11" s="3">
+        <f>U8-U9-U10</f>
+        <v>621</v>
+      </c>
+      <c r="V11" s="3">
+        <f>V8-V9-V10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13">
+        <v>589</v>
+      </c>
+      <c r="O12" s="13">
+        <v>589</v>
+      </c>
+      <c r="P12" s="13">
+        <v>591</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>591</v>
+      </c>
+      <c r="R12" s="13">
+        <v>591</v>
+      </c>
+      <c r="S12" s="13">
+        <v>603</v>
+      </c>
+      <c r="T12" s="13">
+        <v>611</v>
+      </c>
+      <c r="U12" s="13">
+        <v>620</v>
+      </c>
+      <c r="V12" s="13"/>
+    </row>
+    <row r="13" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13">
+        <v>164</v>
+      </c>
+      <c r="O13" s="13">
+        <v>179</v>
+      </c>
+      <c r="P13" s="13">
+        <v>225</v>
+      </c>
+      <c r="Q13" s="13">
+        <v>225</v>
+      </c>
+      <c r="R13" s="13">
+        <v>225</v>
+      </c>
+      <c r="S13" s="13">
+        <v>235</v>
+      </c>
+      <c r="T13" s="13">
+        <v>263</v>
+      </c>
+      <c r="U13" s="13">
+        <v>105</v>
+      </c>
+      <c r="V13" s="13"/>
+    </row>
+    <row r="14" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13">
+        <v>94</v>
+      </c>
+      <c r="O14" s="13">
+        <v>95</v>
+      </c>
+      <c r="P14" s="13">
+        <v>96</v>
+      </c>
+      <c r="Q14" s="13">
+        <v>96</v>
+      </c>
+      <c r="R14" s="13">
+        <v>96</v>
+      </c>
+      <c r="S14" s="13">
+        <v>104</v>
+      </c>
+      <c r="T14" s="13">
+        <v>104</v>
+      </c>
+      <c r="U14" s="13">
+        <v>263</v>
+      </c>
+      <c r="V14" s="13"/>
+    </row>
+    <row r="15" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13">
+        <v>5</v>
+      </c>
+      <c r="O15" s="13">
+        <v>5</v>
+      </c>
+      <c r="P15" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="13">
+        <v>5</v>
+      </c>
+      <c r="R15" s="13">
+        <v>5</v>
+      </c>
+      <c r="S15" s="13">
+        <v>6</v>
+      </c>
+      <c r="T15" s="13">
+        <v>6</v>
+      </c>
+      <c r="U15" s="13">
+        <v>6</v>
+      </c>
+      <c r="V15" s="13"/>
+    </row>
+    <row r="16" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13">
+        <v>24</v>
+      </c>
+      <c r="O16" s="13">
+        <v>29</v>
+      </c>
+      <c r="P16" s="13">
+        <v>31</v>
+      </c>
+      <c r="Q16" s="13">
+        <v>31</v>
+      </c>
+      <c r="R16" s="13">
+        <v>31</v>
+      </c>
+      <c r="S16" s="13">
+        <v>31</v>
+      </c>
+      <c r="T16" s="13">
+        <v>31</v>
+      </c>
+      <c r="U16" s="13">
+        <v>32</v>
+      </c>
+      <c r="V16" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1122,31 +1652,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F33A06-8365-4E68-A964-024E3E0C3481}">
-  <dimension ref="A1:N40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.08984375" customWidth="1"/>
+    <col min="2" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11.1796875" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" customWidth="1"/>
+    <col min="14" max="22" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1189,52 +1720,121 @@
       <c r="N1" s="2">
         <v>43948</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="O1" s="2">
+        <v>43949</v>
+      </c>
+      <c r="P1" s="2">
+        <v>43950</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>43951</v>
+      </c>
+      <c r="R1" s="2">
+        <v>43952</v>
+      </c>
+      <c r="S1" s="2">
+        <v>43953</v>
+      </c>
+      <c r="T1" s="2">
+        <v>43954</v>
+      </c>
+      <c r="U1" s="2">
+        <v>43955</v>
+      </c>
+      <c r="V1" s="2">
+        <v>43956</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="7" customFormat="1" ht="12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7">
+        <f>District!B2</f>
         <v>558</v>
       </c>
       <c r="C2" s="7">
+        <f>District!C2</f>
         <v>575</v>
       </c>
       <c r="D2" s="7">
+        <f>District!D2</f>
         <v>599</v>
       </c>
       <c r="E2" s="7">
+        <f>District!E2</f>
         <v>660</v>
       </c>
       <c r="F2" s="7">
+        <f>District!F2</f>
         <v>690</v>
       </c>
       <c r="G2" s="7">
+        <f>District!G2</f>
         <v>698</v>
       </c>
       <c r="H2" s="7">
+        <f>District!H2</f>
         <v>712</v>
       </c>
       <c r="I2" s="7">
+        <f>District!I2</f>
         <v>726</v>
       </c>
       <c r="J2" s="7">
+        <f>District!J2</f>
         <v>748</v>
       </c>
       <c r="K2" s="7">
+        <f>District!K2</f>
         <v>764</v>
       </c>
       <c r="L2" s="7">
+        <f>District!L2</f>
         <v>772</v>
       </c>
       <c r="M2" s="7">
+        <f>District!M2</f>
         <v>788</v>
       </c>
       <c r="N2" s="7">
+        <f>District!N2</f>
         <v>804</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" s="7">
+        <f>District!O2</f>
+        <v>811</v>
+      </c>
+      <c r="P2" s="7">
+        <f>District!P2</f>
+        <v>828</v>
+      </c>
+      <c r="Q2" s="7">
+        <f>District!Q2</f>
+        <v>840</v>
+      </c>
+      <c r="R2" s="7">
+        <f>District!R2</f>
+        <v>865</v>
+      </c>
+      <c r="S2" s="7">
+        <f>District!S2</f>
+        <v>920</v>
+      </c>
+      <c r="T2" s="7">
+        <f>District!T2</f>
+        <v>935</v>
+      </c>
+      <c r="U2" s="7">
+        <f>District!U2</f>
+        <v>954</v>
+      </c>
+      <c r="V2" s="7">
+        <f>District!V2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1265,8 +1865,30 @@
       <c r="N3" s="5">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="5">
+        <v>78</v>
+      </c>
+      <c r="P3" s="5">
+        <v>82</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>79</v>
+      </c>
+      <c r="R3" s="5">
+        <v>94</v>
+      </c>
+      <c r="S3" s="5">
+        <v>125</v>
+      </c>
+      <c r="T3" s="5">
+        <v>130</v>
+      </c>
+      <c r="U3" s="5">
+        <v>131</v>
+      </c>
+      <c r="V3" s="5"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1297,8 +1919,30 @@
       <c r="N4" s="5">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="5">
+        <v>146</v>
+      </c>
+      <c r="P4" s="5">
+        <v>147</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>147</v>
+      </c>
+      <c r="R4" s="5">
+        <v>147</v>
+      </c>
+      <c r="S4" s="5">
+        <v>152</v>
+      </c>
+      <c r="T4" s="5">
+        <v>154</v>
+      </c>
+      <c r="U4" s="5">
+        <v>155</v>
+      </c>
+      <c r="V4" s="5"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1329,8 +1973,30 @@
       <c r="N5" s="5">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" s="5">
+        <v>55</v>
+      </c>
+      <c r="P5" s="5">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>57</v>
+      </c>
+      <c r="R5" s="5">
+        <v>60</v>
+      </c>
+      <c r="S5" s="5">
+        <v>62</v>
+      </c>
+      <c r="T5" s="5">
+        <v>64</v>
+      </c>
+      <c r="U5" s="5">
+        <v>66</v>
+      </c>
+      <c r="V5" s="5"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -1361,8 +2027,30 @@
       <c r="N6" s="5">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" s="5">
+        <v>51</v>
+      </c>
+      <c r="P6" s="5">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>53</v>
+      </c>
+      <c r="R6" s="5">
+        <v>54</v>
+      </c>
+      <c r="S6" s="5">
+        <v>59</v>
+      </c>
+      <c r="T6" s="5">
+        <v>63</v>
+      </c>
+      <c r="U6" s="5">
+        <v>71</v>
+      </c>
+      <c r="V6" s="5"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1393,8 +2081,30 @@
       <c r="N7" s="5">
         <v>253</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7" s="5">
+        <v>254</v>
+      </c>
+      <c r="P7" s="5">
+        <v>259</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>256</v>
+      </c>
+      <c r="R7" s="5">
+        <v>257</v>
+      </c>
+      <c r="S7" s="5">
+        <v>260</v>
+      </c>
+      <c r="T7" s="5">
+        <v>262</v>
+      </c>
+      <c r="U7" s="5">
+        <v>264</v>
+      </c>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1425,8 +2135,30 @@
       <c r="N8" s="5">
         <v>102</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8" s="5">
+        <v>103</v>
+      </c>
+      <c r="P8" s="5">
+        <v>105</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>104</v>
+      </c>
+      <c r="R8" s="5">
+        <v>106</v>
+      </c>
+      <c r="S8" s="5">
+        <v>108</v>
+      </c>
+      <c r="T8" s="5">
+        <v>108</v>
+      </c>
+      <c r="U8" s="5">
+        <v>109</v>
+      </c>
+      <c r="V8" s="5"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1457,8 +2189,30 @@
       <c r="N9" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9" s="5">
+        <v>57</v>
+      </c>
+      <c r="P9" s="5">
+        <v>59</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>58</v>
+      </c>
+      <c r="R9" s="5">
+        <v>60</v>
+      </c>
+      <c r="S9" s="5">
+        <v>61</v>
+      </c>
+      <c r="T9" s="5">
+        <v>62</v>
+      </c>
+      <c r="U9" s="5">
+        <v>66</v>
+      </c>
+      <c r="V9" s="5"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1489,54 +2243,121 @@
       <c r="N10" s="5">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10" s="5">
+        <v>67</v>
+      </c>
+      <c r="P10" s="5">
+        <v>68</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>86</v>
+      </c>
+      <c r="R10" s="5">
+        <v>87</v>
+      </c>
+      <c r="S10" s="5">
+        <v>93</v>
+      </c>
+      <c r="T10" s="5">
+        <v>92</v>
+      </c>
+      <c r="U10" s="5">
+        <v>92</v>
+      </c>
+      <c r="V10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="7">
+        <f>District!B3</f>
         <v>161</v>
       </c>
       <c r="C11" s="7">
+        <f>District!C3</f>
         <v>180</v>
       </c>
       <c r="D11" s="7">
+        <f>District!D3</f>
         <v>196</v>
       </c>
       <c r="E11" s="7">
+        <f>District!E3</f>
         <v>223</v>
       </c>
       <c r="F11" s="7">
+        <f>District!F3</f>
         <v>233</v>
       </c>
       <c r="G11" s="7">
+        <f>District!G3</f>
         <v>246</v>
       </c>
       <c r="H11" s="7">
+        <f>District!H3</f>
         <v>257</v>
       </c>
       <c r="I11" s="7">
+        <f>District!I3</f>
         <v>265</v>
       </c>
       <c r="J11" s="7">
+        <f>District!J3</f>
         <v>268</v>
       </c>
       <c r="K11" s="7">
+        <f>District!K3</f>
         <v>276</v>
       </c>
       <c r="L11" s="7">
+        <f>District!L3</f>
         <v>287</v>
       </c>
       <c r="M11" s="7">
+        <f>District!M3</f>
         <v>297</v>
       </c>
       <c r="N11" s="7">
+        <f>District!N3</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O11" s="7">
+        <f>District!O3</f>
+        <v>310</v>
+      </c>
+      <c r="P11" s="7">
+        <f>District!P3</f>
+        <v>318</v>
+      </c>
+      <c r="Q11" s="7">
+        <f>District!Q3</f>
+        <v>319</v>
+      </c>
+      <c r="R11" s="7">
+        <f>District!R3</f>
+        <v>328</v>
+      </c>
+      <c r="S11" s="7">
+        <f>District!S3</f>
+        <v>349</v>
+      </c>
+      <c r="T11" s="7">
+        <f>District!T3</f>
+        <v>358</v>
+      </c>
+      <c r="U11" s="7">
+        <f>District!U3</f>
+        <v>360</v>
+      </c>
+      <c r="V11" s="7">
+        <f>District!V3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1565,10 +2386,32 @@
       <c r="N12" s="5">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12" s="5">
+        <v>33</v>
+      </c>
+      <c r="P12" s="5">
+        <v>34</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>33</v>
+      </c>
+      <c r="R12" s="5">
+        <v>33</v>
+      </c>
+      <c r="S12" s="5">
+        <v>33</v>
+      </c>
+      <c r="T12" s="5">
+        <v>34</v>
+      </c>
+      <c r="U12" s="5">
+        <v>36</v>
+      </c>
+      <c r="V12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1577,30 +2420,52 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I13" s="5">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="J13" s="5">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="K13" s="5">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="L13" s="5">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="M13" s="5">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="N13" s="5">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5">
+        <v>29</v>
+      </c>
+      <c r="P13" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>29</v>
+      </c>
+      <c r="R13" s="5">
+        <v>30</v>
+      </c>
+      <c r="S13" s="5">
+        <v>31</v>
+      </c>
+      <c r="T13" s="5">
+        <v>31</v>
+      </c>
+      <c r="U13" s="5">
+        <v>31</v>
+      </c>
+      <c r="V13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1609,30 +2474,52 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5">
+        <v>105</v>
+      </c>
+      <c r="I14" s="5">
+        <v>111</v>
+      </c>
+      <c r="J14" s="5">
+        <v>111</v>
+      </c>
+      <c r="K14" s="5">
+        <v>114</v>
+      </c>
+      <c r="L14" s="5">
+        <v>116</v>
+      </c>
+      <c r="M14" s="5">
+        <v>119</v>
+      </c>
+      <c r="N14" s="5">
+        <v>121</v>
+      </c>
+      <c r="O14" s="5">
+        <v>37</v>
+      </c>
+      <c r="P14" s="5">
+        <v>40</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>38</v>
+      </c>
+      <c r="R14" s="5">
+        <v>42</v>
+      </c>
+      <c r="S14" s="5">
+        <v>69</v>
+      </c>
+      <c r="T14" s="5">
         <v>73</v>
       </c>
-      <c r="I14" s="5">
-        <v>74</v>
-      </c>
-      <c r="J14" s="5">
-        <v>74</v>
-      </c>
-      <c r="K14" s="5">
-        <v>75</v>
-      </c>
-      <c r="L14" s="5">
-        <v>81</v>
-      </c>
-      <c r="M14" s="5">
-        <v>85</v>
-      </c>
-      <c r="N14" s="5">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="U14" s="5">
+        <v>73</v>
+      </c>
+      <c r="V14" s="5"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1641,74 +2528,106 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I15" s="5">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="J15" s="5">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K15" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="L15" s="5">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="M15" s="5">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="N15" s="5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="7">
-        <v>104</v>
-      </c>
-      <c r="C16" s="7">
-        <v>109</v>
-      </c>
-      <c r="D16" s="7">
-        <v>110</v>
-      </c>
-      <c r="E16" s="7">
-        <v>117</v>
-      </c>
-      <c r="F16" s="7">
-        <v>122</v>
-      </c>
-      <c r="G16" s="7">
-        <v>122</v>
-      </c>
-      <c r="H16" s="7">
-        <v>125</v>
-      </c>
-      <c r="I16" s="7">
-        <v>127</v>
-      </c>
-      <c r="J16" s="7">
-        <v>127</v>
-      </c>
-      <c r="K16" s="7">
-        <v>129</v>
-      </c>
-      <c r="L16" s="7">
-        <v>132</v>
-      </c>
-      <c r="M16" s="7">
-        <v>133</v>
-      </c>
-      <c r="N16" s="7">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="5">
+        <v>92</v>
+      </c>
+      <c r="P15" s="5">
+        <v>94</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>92</v>
+      </c>
+      <c r="R15" s="5">
+        <v>94</v>
+      </c>
+      <c r="S15" s="5">
+        <v>94</v>
+      </c>
+      <c r="T15" s="5">
+        <v>94</v>
+      </c>
+      <c r="U15" s="5">
+        <v>94</v>
+      </c>
+      <c r="V15" s="5"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5">
+        <v>73</v>
+      </c>
+      <c r="I16" s="5">
+        <v>74</v>
+      </c>
+      <c r="J16" s="5">
+        <v>74</v>
+      </c>
+      <c r="K16" s="5">
+        <v>75</v>
+      </c>
+      <c r="L16" s="5">
+        <v>81</v>
+      </c>
+      <c r="M16" s="5">
+        <v>85</v>
+      </c>
+      <c r="N16" s="5">
+        <v>86</v>
+      </c>
+      <c r="O16" s="5">
+        <v>77</v>
+      </c>
+      <c r="P16" s="5">
+        <v>79</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>77</v>
+      </c>
+      <c r="R16" s="5">
+        <v>77</v>
+      </c>
+      <c r="S16" s="5">
+        <v>78</v>
+      </c>
+      <c r="T16" s="5">
+        <v>81</v>
+      </c>
+      <c r="U16" s="5">
+        <v>81</v>
+      </c>
+      <c r="V16" s="5"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1717,30 +2636,52 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I17" s="5">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="J17" s="5">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K17" s="5">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L17" s="5">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="M17" s="5">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="N17" s="5">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O17" s="5">
+        <v>10</v>
+      </c>
+      <c r="P17" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>10</v>
+      </c>
+      <c r="R17" s="5">
+        <v>10</v>
+      </c>
+      <c r="S17" s="5">
+        <v>10</v>
+      </c>
+      <c r="T17" s="5">
+        <v>10</v>
+      </c>
+      <c r="U17" s="5">
+        <v>10</v>
+      </c>
+      <c r="V17" s="5"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1749,62 +2690,141 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I18" s="5">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="J18" s="5">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="K18" s="5">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="L18" s="5">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="M18" s="5">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="N18" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5">
-        <v>15</v>
-      </c>
-      <c r="I19" s="5">
-        <v>15</v>
-      </c>
-      <c r="J19" s="5">
-        <v>16</v>
-      </c>
-      <c r="K19" s="5">
-        <v>16</v>
-      </c>
-      <c r="L19" s="5">
-        <v>16</v>
-      </c>
-      <c r="M19" s="5">
-        <v>16</v>
-      </c>
-      <c r="N19" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="O18" s="5">
+        <v>32</v>
+      </c>
+      <c r="P18" s="5">
+        <v>31</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>40</v>
+      </c>
+      <c r="R18" s="5">
+        <v>42</v>
+      </c>
+      <c r="S18" s="5">
+        <v>34</v>
+      </c>
+      <c r="T18" s="5">
+        <v>35</v>
+      </c>
+      <c r="U18" s="5">
+        <v>35</v>
+      </c>
+      <c r="V18" s="5"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="7">
+        <f>District!B4</f>
+        <v>104</v>
+      </c>
+      <c r="C19" s="7">
+        <f>District!C4</f>
+        <v>109</v>
+      </c>
+      <c r="D19" s="7">
+        <f>District!D4</f>
+        <v>110</v>
+      </c>
+      <c r="E19" s="7">
+        <f>District!E4</f>
+        <v>117</v>
+      </c>
+      <c r="F19" s="7">
+        <f>District!F4</f>
+        <v>122</v>
+      </c>
+      <c r="G19" s="7">
+        <f>District!G4</f>
+        <v>122</v>
+      </c>
+      <c r="H19" s="7">
+        <f>District!H4</f>
+        <v>125</v>
+      </c>
+      <c r="I19" s="7">
+        <f>District!I4</f>
+        <v>127</v>
+      </c>
+      <c r="J19" s="7">
+        <f>District!J4</f>
+        <v>127</v>
+      </c>
+      <c r="K19" s="7">
+        <f>District!K4</f>
+        <v>129</v>
+      </c>
+      <c r="L19" s="7">
+        <f>District!L4</f>
+        <v>132</v>
+      </c>
+      <c r="M19" s="7">
+        <f>District!M4</f>
+        <v>133</v>
+      </c>
+      <c r="N19" s="7">
+        <f>District!N4</f>
+        <v>136</v>
+      </c>
+      <c r="O19" s="7">
+        <f>District!O4</f>
+        <v>144</v>
+      </c>
+      <c r="P19" s="7">
+        <f>District!P4</f>
+        <v>149</v>
+      </c>
+      <c r="Q19" s="7">
+        <f>District!Q4</f>
+        <v>172</v>
+      </c>
+      <c r="R19" s="7">
+        <f>District!R4</f>
+        <v>187</v>
+      </c>
+      <c r="S19" s="7">
+        <f>District!S4</f>
+        <v>201</v>
+      </c>
+      <c r="T19" s="7">
+        <f>District!T4</f>
+        <v>201</v>
+      </c>
+      <c r="U19" s="7">
+        <f>District!U4</f>
+        <v>211</v>
+      </c>
+      <c r="V19" s="7">
+        <f>District!V4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1813,30 +2833,52 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I20" s="5">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="J20" s="5">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="K20" s="5">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="L20" s="5">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="M20" s="5">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="N20" s="5">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="O20" s="5">
+        <v>29</v>
+      </c>
+      <c r="P20" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>30</v>
+      </c>
+      <c r="R20" s="5">
+        <v>30</v>
+      </c>
+      <c r="S20" s="5">
+        <v>31</v>
+      </c>
+      <c r="T20" s="5">
+        <v>31</v>
+      </c>
+      <c r="U20" s="5">
+        <v>32</v>
+      </c>
+      <c r="V20" s="5"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1845,30 +2887,52 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I21" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J21" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K21" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L21" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M21" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N21" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="O21" s="5">
+        <v>4</v>
+      </c>
+      <c r="P21" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>4</v>
+      </c>
+      <c r="R21" s="5">
+        <v>4</v>
+      </c>
+      <c r="S21" s="5">
+        <v>4</v>
+      </c>
+      <c r="T21" s="5">
+        <v>4</v>
+      </c>
+      <c r="U21" s="5">
+        <v>4</v>
+      </c>
+      <c r="V21" s="5"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1877,30 +2941,52 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="I22" s="5">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="J22" s="5">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="K22" s="5">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L22" s="5">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M22" s="5">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="N22" s="5">
+        <v>16</v>
+      </c>
+      <c r="O22" s="5">
+        <v>23</v>
+      </c>
+      <c r="P22" s="5">
+        <v>23</v>
+      </c>
+      <c r="Q22" s="5">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="R22" s="5">
+        <v>53</v>
+      </c>
+      <c r="S22" s="5">
+        <v>58</v>
+      </c>
+      <c r="T22" s="5">
+        <v>58</v>
+      </c>
+      <c r="U22" s="5">
+        <v>59</v>
+      </c>
+      <c r="V22" s="5"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1909,30 +2995,52 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="I23" s="5">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="J23" s="5">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="K23" s="5">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="L23" s="5">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="M23" s="5">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="N23" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="O23" s="5">
+        <v>44</v>
+      </c>
+      <c r="P23" s="5">
+        <v>44</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>47</v>
+      </c>
+      <c r="R23" s="5">
+        <v>50</v>
+      </c>
+      <c r="S23" s="5">
+        <v>53</v>
+      </c>
+      <c r="T23" s="5">
+        <v>53</v>
+      </c>
+      <c r="U23" s="5">
+        <v>55</v>
+      </c>
+      <c r="V23" s="5"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1941,74 +3049,106 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I24" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J24" s="5">
         <v>1</v>
       </c>
       <c r="K24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="7">
-        <v>8</v>
-      </c>
-      <c r="C25" s="7">
-        <v>8</v>
-      </c>
-      <c r="D25" s="7">
-        <v>10</v>
-      </c>
-      <c r="E25" s="7">
-        <v>10</v>
-      </c>
-      <c r="F25" s="7">
-        <v>11</v>
-      </c>
-      <c r="G25" s="7">
-        <v>11</v>
-      </c>
-      <c r="H25" s="7">
-        <v>11</v>
-      </c>
-      <c r="I25" s="7">
-        <v>11</v>
-      </c>
-      <c r="J25" s="7">
-        <v>13</v>
-      </c>
-      <c r="K25" s="7">
-        <v>15</v>
-      </c>
-      <c r="L25" s="7">
-        <v>15</v>
-      </c>
-      <c r="M25" s="7">
-        <v>15</v>
-      </c>
-      <c r="N25" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O24" s="5">
+        <v>1</v>
+      </c>
+      <c r="P24" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>1</v>
+      </c>
+      <c r="R24" s="5">
+        <v>1</v>
+      </c>
+      <c r="S24" s="5">
+        <v>3</v>
+      </c>
+      <c r="T24" s="5">
+        <v>3</v>
+      </c>
+      <c r="U24" s="5">
+        <v>3</v>
+      </c>
+      <c r="V24" s="5"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5">
+        <v>37</v>
+      </c>
+      <c r="I25" s="5">
+        <v>38</v>
+      </c>
+      <c r="J25" s="5">
+        <v>39</v>
+      </c>
+      <c r="K25" s="5">
+        <v>40</v>
+      </c>
+      <c r="L25" s="5">
+        <v>40</v>
+      </c>
+      <c r="M25" s="5">
+        <v>40</v>
+      </c>
+      <c r="N25" s="5">
+        <v>42</v>
+      </c>
+      <c r="O25" s="5">
+        <v>42</v>
+      </c>
+      <c r="P25" s="5">
+        <v>42</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>43</v>
+      </c>
+      <c r="R25" s="5">
+        <v>44</v>
+      </c>
+      <c r="S25" s="5">
+        <v>45</v>
+      </c>
+      <c r="T25" s="5">
+        <v>45</v>
+      </c>
+      <c r="U25" s="5">
+        <v>47</v>
+      </c>
+      <c r="V25" s="5"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2017,30 +3157,52 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N26" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O26" s="5">
+        <v>1</v>
+      </c>
+      <c r="P26" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>1</v>
+      </c>
+      <c r="R26" s="5">
+        <v>1</v>
+      </c>
+      <c r="S26" s="5">
+        <v>1</v>
+      </c>
+      <c r="T26" s="5">
+        <v>1</v>
+      </c>
+      <c r="U26" s="5">
+        <v>5</v>
+      </c>
+      <c r="V26" s="5"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2049,62 +3211,141 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I27" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J27" s="5">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K27" s="5">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5">
+        <v>0</v>
+      </c>
+      <c r="M27" s="5">
+        <v>0</v>
+      </c>
+      <c r="N27" s="5">
+        <v>0</v>
+      </c>
+      <c r="O27" s="5">
+        <v>0</v>
+      </c>
+      <c r="P27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="5">
+        <v>4</v>
+      </c>
+      <c r="R27" s="5">
+        <v>4</v>
+      </c>
+      <c r="S27" s="5">
+        <v>6</v>
+      </c>
+      <c r="T27" s="5">
+        <v>6</v>
+      </c>
+      <c r="U27" s="5">
+        <v>6</v>
+      </c>
+      <c r="V27" s="5"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="7">
+        <f>District!B5</f>
+        <v>8</v>
+      </c>
+      <c r="C28" s="7">
+        <f>District!C5</f>
+        <v>8</v>
+      </c>
+      <c r="D28" s="7">
+        <f>District!D5</f>
+        <v>10</v>
+      </c>
+      <c r="E28" s="7">
+        <f>District!E5</f>
+        <v>10</v>
+      </c>
+      <c r="F28" s="7">
+        <f>District!F5</f>
         <v>11</v>
       </c>
-      <c r="L27" s="5">
+      <c r="G28" s="7">
+        <f>District!G5</f>
         <v>11</v>
       </c>
-      <c r="M27" s="5">
+      <c r="H28" s="7">
+        <f>District!H5</f>
         <v>11</v>
       </c>
-      <c r="N27" s="5">
+      <c r="I28" s="7">
+        <f>District!I5</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5">
-        <v>0</v>
-      </c>
-      <c r="I28" s="5">
-        <v>0</v>
-      </c>
-      <c r="J28" s="5">
-        <v>0</v>
-      </c>
-      <c r="K28" s="5">
-        <v>0</v>
-      </c>
-      <c r="L28" s="5">
-        <v>0</v>
-      </c>
-      <c r="M28" s="5">
-        <v>0</v>
-      </c>
-      <c r="N28" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J28" s="7">
+        <f>District!J5</f>
+        <v>13</v>
+      </c>
+      <c r="K28" s="7">
+        <f>District!K5</f>
+        <v>15</v>
+      </c>
+      <c r="L28" s="7">
+        <f>District!L5</f>
+        <v>15</v>
+      </c>
+      <c r="M28" s="7">
+        <f>District!M5</f>
+        <v>15</v>
+      </c>
+      <c r="N28" s="7">
+        <f>District!N5</f>
+        <v>15</v>
+      </c>
+      <c r="O28" s="7">
+        <f>District!O5</f>
+        <v>15</v>
+      </c>
+      <c r="P28" s="7">
+        <f>District!P5</f>
+        <v>16</v>
+      </c>
+      <c r="Q28" s="7">
+        <f>District!Q5</f>
+        <v>16</v>
+      </c>
+      <c r="R28" s="7">
+        <f>District!R5</f>
+        <v>18</v>
+      </c>
+      <c r="S28" s="7">
+        <f>District!S5</f>
+        <v>19</v>
+      </c>
+      <c r="T28" s="7">
+        <f>District!T5</f>
+        <v>21</v>
+      </c>
+      <c r="U28" s="7">
+        <f>District!U5</f>
+        <v>21</v>
+      </c>
+      <c r="V28" s="7">
+        <f>District!V5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2113,10 +3354,10 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I29" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J29" s="5">
         <v>2</v>
@@ -2131,56 +3372,88 @@
         <v>2</v>
       </c>
       <c r="N29" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="7">
-        <v>35</v>
-      </c>
-      <c r="C30" s="7">
-        <v>35</v>
-      </c>
-      <c r="D30" s="7">
-        <v>35</v>
-      </c>
-      <c r="E30" s="7">
-        <v>38</v>
-      </c>
-      <c r="F30" s="7">
-        <v>39</v>
-      </c>
-      <c r="G30" s="7">
-        <v>39</v>
-      </c>
-      <c r="H30" s="7">
-        <v>40</v>
-      </c>
-      <c r="I30" s="7">
-        <v>41</v>
-      </c>
-      <c r="J30" s="7">
-        <v>42</v>
-      </c>
-      <c r="K30" s="7">
-        <v>42</v>
-      </c>
-      <c r="L30" s="7">
-        <v>42</v>
-      </c>
-      <c r="M30" s="7">
-        <v>43</v>
-      </c>
-      <c r="N30" s="7">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="O29" s="5">
+        <v>3</v>
+      </c>
+      <c r="P29" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q29" s="5">
+        <v>3</v>
+      </c>
+      <c r="R29" s="5">
+        <v>3</v>
+      </c>
+      <c r="S29" s="5">
+        <v>3</v>
+      </c>
+      <c r="T29" s="5">
+        <v>3</v>
+      </c>
+      <c r="U29" s="5">
+        <v>3</v>
+      </c>
+      <c r="V29" s="5"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5">
+        <v>9</v>
+      </c>
+      <c r="I30" s="5">
+        <v>9</v>
+      </c>
+      <c r="J30" s="5">
+        <v>9</v>
+      </c>
+      <c r="K30" s="5">
+        <v>11</v>
+      </c>
+      <c r="L30" s="5">
+        <v>11</v>
+      </c>
+      <c r="M30" s="5">
+        <v>11</v>
+      </c>
+      <c r="N30" s="5">
+        <v>11</v>
+      </c>
+      <c r="O30" s="5">
+        <v>11</v>
+      </c>
+      <c r="P30" s="5">
+        <v>12</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>12</v>
+      </c>
+      <c r="R30" s="5">
+        <v>14</v>
+      </c>
+      <c r="S30" s="5">
+        <v>14</v>
+      </c>
+      <c r="T30" s="5">
+        <v>14</v>
+      </c>
+      <c r="U30" s="5">
+        <v>14</v>
+      </c>
+      <c r="V30" s="5"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2189,30 +3462,52 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I31" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J31" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K31" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="L31" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M31" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="N31" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P31" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>1</v>
+      </c>
+      <c r="R31" s="5">
+        <v>1</v>
+      </c>
+      <c r="S31" s="5">
+        <v>2</v>
+      </c>
+      <c r="T31" s="5">
+        <v>4</v>
+      </c>
+      <c r="U31" s="5">
+        <v>4</v>
+      </c>
+      <c r="V31" s="5"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2221,62 +3516,141 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I32" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J32" s="5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K32" s="5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L32" s="5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="M32" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N32" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5">
-        <v>2</v>
-      </c>
-      <c r="I33" s="5">
-        <v>2</v>
-      </c>
-      <c r="J33" s="5">
-        <v>2</v>
-      </c>
-      <c r="K33" s="5">
-        <v>2</v>
-      </c>
-      <c r="L33" s="5">
-        <v>2</v>
-      </c>
-      <c r="M33" s="5">
-        <v>2</v>
-      </c>
-      <c r="N33" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O32" s="5">
+        <v>0</v>
+      </c>
+      <c r="P32" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="5">
+        <v>0</v>
+      </c>
+      <c r="R32" s="5">
+        <v>0</v>
+      </c>
+      <c r="S32" s="5">
+        <v>0</v>
+      </c>
+      <c r="T32" s="5">
+        <v>0</v>
+      </c>
+      <c r="U32" s="5">
+        <v>0</v>
+      </c>
+      <c r="V32" s="5"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="7">
+        <f>District!B6</f>
+        <v>35</v>
+      </c>
+      <c r="C33" s="7">
+        <f>District!C6</f>
+        <v>35</v>
+      </c>
+      <c r="D33" s="7">
+        <f>District!D6</f>
+        <v>35</v>
+      </c>
+      <c r="E33" s="7">
+        <f>District!E6</f>
+        <v>38</v>
+      </c>
+      <c r="F33" s="7">
+        <f>District!F6</f>
+        <v>39</v>
+      </c>
+      <c r="G33" s="7">
+        <f>District!G6</f>
+        <v>39</v>
+      </c>
+      <c r="H33" s="7">
+        <f>District!H6</f>
+        <v>40</v>
+      </c>
+      <c r="I33" s="7">
+        <f>District!I6</f>
+        <v>41</v>
+      </c>
+      <c r="J33" s="7">
+        <f>District!J6</f>
+        <v>42</v>
+      </c>
+      <c r="K33" s="7">
+        <f>District!K6</f>
+        <v>42</v>
+      </c>
+      <c r="L33" s="7">
+        <f>District!L6</f>
+        <v>42</v>
+      </c>
+      <c r="M33" s="7">
+        <f>District!M6</f>
+        <v>43</v>
+      </c>
+      <c r="N33" s="7">
+        <f>District!N6</f>
+        <v>43</v>
+      </c>
+      <c r="O33" s="7">
+        <f>District!O6</f>
+        <v>43</v>
+      </c>
+      <c r="P33" s="7">
+        <f>District!P6</f>
+        <v>43</v>
+      </c>
+      <c r="Q33" s="7">
+        <f>District!Q6</f>
+        <v>44</v>
+      </c>
+      <c r="R33" s="7">
+        <f>District!R6</f>
+        <v>45</v>
+      </c>
+      <c r="S33" s="7">
+        <f>District!S6</f>
+        <v>45</v>
+      </c>
+      <c r="T33" s="7">
+        <f>District!T6</f>
+        <v>45</v>
+      </c>
+      <c r="U33" s="7">
+        <f>District!U6</f>
+        <v>51</v>
+      </c>
+      <c r="V33" s="7">
+        <f>District!V6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2285,236 +3659,679 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I34" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J34" s="5">
+        <v>30</v>
+      </c>
+      <c r="K34" s="5">
+        <v>30</v>
+      </c>
+      <c r="L34" s="5">
+        <v>30</v>
+      </c>
+      <c r="M34" s="5">
+        <v>30</v>
+      </c>
+      <c r="N34" s="5">
+        <v>30</v>
+      </c>
+      <c r="O34" s="5">
+        <v>30</v>
+      </c>
+      <c r="P34" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q34" s="5">
+        <v>31</v>
+      </c>
+      <c r="R34" s="5">
+        <v>31</v>
+      </c>
+      <c r="S34" s="5">
+        <v>31</v>
+      </c>
+      <c r="T34" s="5">
+        <v>31</v>
+      </c>
+      <c r="U34" s="5">
+        <v>36</v>
+      </c>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5">
+        <v>8</v>
+      </c>
+      <c r="I35" s="5">
+        <v>9</v>
+      </c>
+      <c r="J35" s="5">
+        <v>9</v>
+      </c>
+      <c r="K35" s="5">
+        <v>9</v>
+      </c>
+      <c r="L35" s="5">
+        <v>9</v>
+      </c>
+      <c r="M35" s="5">
+        <v>10</v>
+      </c>
+      <c r="N35" s="5">
+        <v>10</v>
+      </c>
+      <c r="O35" s="5">
+        <v>10</v>
+      </c>
+      <c r="P35" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q35" s="5">
+        <v>10</v>
+      </c>
+      <c r="R35" s="5">
+        <v>10</v>
+      </c>
+      <c r="S35" s="5">
+        <v>10</v>
+      </c>
+      <c r="T35" s="5">
+        <v>10</v>
+      </c>
+      <c r="U35" s="5">
+        <v>10</v>
+      </c>
+      <c r="V35" s="5"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5">
+        <v>2</v>
+      </c>
+      <c r="I36" s="5">
+        <v>2</v>
+      </c>
+      <c r="J36" s="5">
+        <v>2</v>
+      </c>
+      <c r="K36" s="5">
+        <v>2</v>
+      </c>
+      <c r="L36" s="5">
+        <v>2</v>
+      </c>
+      <c r="M36" s="5">
+        <v>2</v>
+      </c>
+      <c r="N36" s="5">
+        <v>2</v>
+      </c>
+      <c r="O36" s="5">
+        <v>2</v>
+      </c>
+      <c r="P36" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>2</v>
+      </c>
+      <c r="R36" s="5">
+        <v>3</v>
+      </c>
+      <c r="S36" s="5">
+        <v>3</v>
+      </c>
+      <c r="T36" s="5">
+        <v>3</v>
+      </c>
+      <c r="U36" s="5">
+        <v>3</v>
+      </c>
+      <c r="V36" s="5"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A37" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
+      <c r="I37" s="10">
+        <v>0</v>
+      </c>
+      <c r="J37" s="10">
         <v>1</v>
       </c>
-      <c r="K34" s="5">
+      <c r="K37" s="10">
         <v>1</v>
       </c>
-      <c r="L34" s="5">
+      <c r="L37" s="10">
         <v>1</v>
       </c>
-      <c r="M34" s="5">
+      <c r="M37" s="10">
         <v>1</v>
       </c>
-      <c r="N34" s="5">
+      <c r="N37" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="O37" s="10">
+        <v>1</v>
+      </c>
+      <c r="P37" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="10">
+        <v>1</v>
+      </c>
+      <c r="R37" s="10">
+        <v>1</v>
+      </c>
+      <c r="S37" s="10">
+        <v>1</v>
+      </c>
+      <c r="T37" s="10">
+        <v>1</v>
+      </c>
+      <c r="U37" s="10">
+        <v>2</v>
+      </c>
+      <c r="V37" s="10"/>
+    </row>
+    <row r="38" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B38" s="11">
+        <f>District!B7</f>
         <v>64</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C38" s="11">
+        <f>District!C7</f>
         <v>62</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D38" s="11">
+        <f>District!D7</f>
         <v>68</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E38" s="11">
+        <f>District!E7</f>
         <v>53</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F38" s="11">
+        <f>District!F7</f>
         <v>53</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G38" s="11">
+        <f>District!G7</f>
         <v>54</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H38" s="11">
+        <f>District!H7</f>
         <v>54</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I38" s="11">
+        <f>District!I7</f>
         <v>54</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J38" s="11">
+        <f>District!J7</f>
         <v>54</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K38" s="11">
+        <f>District!K7</f>
         <v>55</v>
       </c>
-      <c r="L35" s="1">
+      <c r="L38" s="11">
+        <f>District!L7</f>
         <v>56</v>
       </c>
-      <c r="M35" s="1">
+      <c r="M38" s="11">
+        <f>District!M7</f>
         <v>55</v>
       </c>
-      <c r="N35" s="1">
+      <c r="N38" s="11">
+        <f>District!N7</f>
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="O38" s="11">
+        <f>District!O7</f>
+        <v>54</v>
+      </c>
+      <c r="P38" s="11">
+        <f>District!P7</f>
+        <v>54</v>
+      </c>
+      <c r="Q38" s="11">
+        <f>District!Q7</f>
+        <v>55</v>
+      </c>
+      <c r="R38" s="11">
+        <f>District!R7</f>
+        <v>64</v>
+      </c>
+      <c r="S38" s="11">
+        <f>District!S7</f>
+        <v>64</v>
+      </c>
+      <c r="T38" s="11">
+        <f>District!T7</f>
+        <v>64</v>
+      </c>
+      <c r="U38" s="11">
+        <f>District!U7</f>
+        <v>64</v>
+      </c>
+      <c r="V38" s="11">
+        <f>District!V7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B39" s="11">
+        <f>District!B8</f>
         <v>930</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C39" s="11">
+        <f>District!C8</f>
         <v>969</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D39" s="11">
+        <f>District!D8</f>
         <v>1018</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E39" s="11">
+        <f>District!E8</f>
         <v>1101</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F39" s="11">
+        <f>District!F8</f>
         <v>1148</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G39" s="11">
+        <f>District!G8</f>
         <v>1170</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H39" s="11">
+        <f>District!H8</f>
         <v>1199</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I39" s="11">
+        <f>District!I8</f>
         <v>1224</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J39" s="11">
+        <f>District!J8</f>
         <v>1252</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K39" s="11">
+        <f>District!K8</f>
         <v>1281</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L39" s="11">
+        <f>District!L8</f>
         <v>1304</v>
       </c>
-      <c r="M36" s="3">
+      <c r="M39" s="11">
+        <f>District!M8</f>
         <v>1331</v>
       </c>
-      <c r="N36" s="3">
+      <c r="N39" s="11">
+        <f>District!N8</f>
         <v>1353</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="O39" s="11">
+        <f>District!O8</f>
+        <v>1377</v>
+      </c>
+      <c r="P39" s="11">
+        <f>District!P8</f>
+        <v>1408</v>
+      </c>
+      <c r="Q39" s="11">
+        <f>District!Q8</f>
+        <v>1446</v>
+      </c>
+      <c r="R39" s="11">
+        <f>District!R8</f>
+        <v>1507</v>
+      </c>
+      <c r="S39" s="11">
+        <f>District!S8</f>
+        <v>1598</v>
+      </c>
+      <c r="T39" s="11">
+        <f>District!T8</f>
+        <v>1624</v>
+      </c>
+      <c r="U39" s="11">
+        <f>District!U8</f>
+        <v>1661</v>
+      </c>
+      <c r="V39" s="11">
+        <f>District!V8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B40" s="11">
+        <f>District!B9</f>
         <v>5</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C40" s="11">
+        <f>District!C9</f>
         <v>6</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D40" s="11">
+        <f>District!D9</f>
         <v>6</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E40" s="11">
+        <f>District!E9</f>
         <v>6</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F40" s="11">
+        <f>District!F9</f>
         <v>6</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G40" s="11">
+        <f>District!G9</f>
         <v>7</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H40" s="11">
+        <f>District!H9</f>
         <v>7</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I40" s="11">
+        <f>District!I9</f>
         <v>7</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J40" s="11">
+        <f>District!J9</f>
         <v>8</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K40" s="11">
+        <f>District!K9</f>
         <v>8</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L40" s="11">
+        <f>District!L9</f>
         <v>8</v>
       </c>
-      <c r="M37" s="3">
+      <c r="M40" s="11">
+        <f>District!M9</f>
         <v>8</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N40" s="11">
+        <f>District!N9</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="O40" s="11">
+        <f>District!O9</f>
+        <v>8</v>
+      </c>
+      <c r="P40" s="11">
+        <f>District!P9</f>
+        <v>11</v>
+      </c>
+      <c r="Q40" s="11">
+        <f>District!Q9</f>
+        <v>11</v>
+      </c>
+      <c r="R40" s="11">
+        <f>District!R9</f>
+        <v>12</v>
+      </c>
+      <c r="S40" s="11">
+        <f>District!S9</f>
+        <v>12</v>
+      </c>
+      <c r="T40" s="11">
+        <f>District!T9</f>
+        <v>14</v>
+      </c>
+      <c r="U40" s="11">
+        <f>District!U9</f>
+        <v>14</v>
+      </c>
+      <c r="V40" s="11">
+        <f>District!V9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B41" s="11">
+        <f>District!B10</f>
         <v>479</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C41" s="11">
+        <f>District!C10</f>
         <v>479</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D41" s="11">
+        <f>District!D10</f>
         <v>540</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E41" s="11">
+        <f>District!E10</f>
         <v>545</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F41" s="11">
+        <f>District!F10</f>
         <v>551</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G41" s="11">
+        <f>District!G10</f>
         <v>574</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H41" s="11">
+        <f>District!H10</f>
         <v>781</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I41" s="11">
+        <f>District!I10</f>
         <v>826</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J41" s="11">
+        <f>District!J10</f>
         <v>843</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K41" s="11">
+        <f>District!K10</f>
         <v>846</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L41" s="11">
+        <f>District!L10</f>
         <v>855</v>
       </c>
-      <c r="M38" s="3">
+      <c r="M41" s="11">
+        <f>District!M10</f>
         <v>868</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N41" s="11">
+        <f>District!N10</f>
         <v>876</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="O41" s="11">
+        <f>District!O10</f>
+        <v>897</v>
+      </c>
+      <c r="P41" s="11">
+        <f>District!P10</f>
+        <v>897</v>
+      </c>
+      <c r="Q41" s="11">
+        <f>District!Q10</f>
+        <v>948</v>
+      </c>
+      <c r="R41" s="11">
+        <f>District!R10</f>
+        <v>948</v>
+      </c>
+      <c r="S41" s="11">
+        <f>District!S10</f>
+        <v>979</v>
+      </c>
+      <c r="T41" s="11">
+        <f>District!T10</f>
+        <v>1015</v>
+      </c>
+      <c r="U41" s="11">
+        <f>District!U10</f>
+        <v>1026</v>
+      </c>
+      <c r="V41" s="11">
+        <f>District!V10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
+      <c r="B42" s="11">
+        <f>District!B11</f>
+        <v>446</v>
+      </c>
+      <c r="C42" s="11">
+        <f>District!C11</f>
+        <v>484</v>
+      </c>
+      <c r="D42" s="11">
+        <f>District!D11</f>
+        <v>472</v>
+      </c>
+      <c r="E42" s="11">
+        <f>District!E11</f>
+        <v>550</v>
+      </c>
+      <c r="F42" s="11">
+        <f>District!F11</f>
+        <v>591</v>
+      </c>
+      <c r="G42" s="11">
+        <f>District!G11</f>
+        <v>589</v>
+      </c>
+      <c r="H42" s="11">
+        <f>District!H11</f>
+        <v>411</v>
+      </c>
+      <c r="I42" s="11">
+        <f>District!I11</f>
+        <v>391</v>
+      </c>
+      <c r="J42" s="11">
+        <f>District!J11</f>
+        <v>401</v>
+      </c>
+      <c r="K42" s="11">
+        <f>District!K11</f>
+        <v>427</v>
+      </c>
+      <c r="L42" s="11">
+        <f>District!L11</f>
+        <v>441</v>
+      </c>
+      <c r="M42" s="11">
+        <f>District!M11</f>
+        <v>455</v>
+      </c>
+      <c r="N42" s="11">
+        <f>District!N11</f>
+        <v>469</v>
+      </c>
+      <c r="O42" s="11">
+        <f>District!O11</f>
+        <v>472</v>
+      </c>
+      <c r="P42" s="11">
+        <f>District!P11</f>
+        <v>500</v>
+      </c>
+      <c r="Q42" s="11">
+        <f>District!Q11</f>
+        <v>487</v>
+      </c>
+      <c r="R42" s="11">
+        <f>District!R11</f>
+        <v>547</v>
+      </c>
+      <c r="S42" s="11">
+        <f>District!S11</f>
+        <v>607</v>
+      </c>
+      <c r="T42" s="11">
+        <f>District!T11</f>
+        <v>595</v>
+      </c>
+      <c r="U42" s="11">
+        <f>District!U11</f>
+        <v>621</v>
+      </c>
+      <c r="V42" s="11">
+        <f>District!V11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12"/>
+      <c r="S43" s="12"/>
+      <c r="T43" s="12"/>
+      <c r="U43" s="12"/>
+      <c r="V43" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -2524,20 +4341,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7EDF83-9869-4E9A-880E-E93BD53C3AC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C44669B21B127D45AF6F62C9A293CCC7" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a3b65afc6cbe717343e4256a9fdd90e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="04f85633-9dbd-493d-9c0a-002b900dde1c" xmlns:ns4="1f157ad2-2ae5-4763-9ea7-a4403f644984" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="de83bd4fc27362efc22842edd0fa359c" ns3:_="" ns4:_="">
     <xsd:import namespace="04f85633-9dbd-493d-9c0a-002b900dde1c"/>
@@ -2754,15 +4580,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2770,6 +4587,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F13BE49F-5AB0-4CF9-A4E6-9B8400ED2BB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B495C0-610E-423A-AAC4-17117BBB3EAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2788,14 +4613,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F13BE49F-5AB0-4CF9-A4E6-9B8400ED2BB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51454EB7-2533-4710-B1B7-84600D145D91}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update with data from 05/05/2020
</commit_message>
<xml_diff>
--- a/Data/Covid2019/SA_data_archive/Gauteng/Covid 19 Data.xlsx
+++ b/Data/Covid2019/SA_data_archive/Gauteng/Covid 19 Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="District" sheetId="1" r:id="rId1"/>
@@ -653,7 +653,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -663,9 +663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S21" sqref="S21"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -822,6 +822,9 @@
       <c r="U2">
         <v>954</v>
       </c>
+      <c r="V2">
+        <v>971</v>
+      </c>
     </row>
     <row r="3" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -887,6 +890,9 @@
       <c r="U3">
         <v>360</v>
       </c>
+      <c r="V3">
+        <v>366</v>
+      </c>
     </row>
     <row r="4" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -952,6 +958,9 @@
       <c r="U4">
         <v>211</v>
       </c>
+      <c r="V4">
+        <v>224</v>
+      </c>
     </row>
     <row r="5" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1017,6 +1026,9 @@
       <c r="U5">
         <v>21</v>
       </c>
+      <c r="V5">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1082,6 +1094,9 @@
       <c r="U6">
         <v>51</v>
       </c>
+      <c r="V6">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1147,6 +1162,9 @@
       <c r="U7">
         <v>64</v>
       </c>
+      <c r="V7">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
@@ -1212,7 +1230,9 @@
       <c r="U8" s="3">
         <v>1661</v>
       </c>
-      <c r="V8" s="3"/>
+      <c r="V8" s="3">
+        <v>1697</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -1278,7 +1298,9 @@
       <c r="U9" s="3">
         <v>14</v>
       </c>
-      <c r="V9" s="3"/>
+      <c r="V9" s="3">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -1344,95 +1366,97 @@
       <c r="U10" s="3">
         <v>1026</v>
       </c>
-      <c r="V10" s="3"/>
+      <c r="V10" s="3">
+        <v>1036</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <f>B8-B9-B10</f>
+        <f t="shared" ref="B11:V11" si="0">B8-B9-B10</f>
         <v>446</v>
       </c>
       <c r="C11" s="3">
-        <f>C8-C9-C10</f>
+        <f t="shared" si="0"/>
         <v>484</v>
       </c>
       <c r="D11" s="3">
-        <f>D8-D9-D10</f>
+        <f t="shared" si="0"/>
         <v>472</v>
       </c>
       <c r="E11" s="3">
-        <f>E8-E9-E10</f>
+        <f t="shared" si="0"/>
         <v>550</v>
       </c>
       <c r="F11" s="3">
-        <f>F8-F9-F10</f>
+        <f t="shared" si="0"/>
         <v>591</v>
       </c>
       <c r="G11" s="3">
-        <f>G8-G9-G10</f>
+        <f t="shared" si="0"/>
         <v>589</v>
       </c>
       <c r="H11" s="3">
-        <f>H8-H9-H10</f>
+        <f t="shared" si="0"/>
         <v>411</v>
       </c>
       <c r="I11" s="3">
-        <f>I8-I9-I10</f>
+        <f t="shared" si="0"/>
         <v>391</v>
       </c>
       <c r="J11" s="3">
-        <f>J8-J9-J10</f>
+        <f t="shared" si="0"/>
         <v>401</v>
       </c>
       <c r="K11" s="3">
-        <f>K8-K9-K10</f>
+        <f t="shared" si="0"/>
         <v>427</v>
       </c>
       <c r="L11" s="3">
-        <f>L8-L9-L10</f>
+        <f t="shared" si="0"/>
         <v>441</v>
       </c>
       <c r="M11" s="3">
-        <f>M8-M9-M10</f>
+        <f t="shared" si="0"/>
         <v>455</v>
       </c>
       <c r="N11" s="3">
-        <f>N8-N9-N10</f>
+        <f t="shared" si="0"/>
         <v>469</v>
       </c>
       <c r="O11" s="3">
-        <f>O8-O9-O10</f>
+        <f t="shared" si="0"/>
         <v>472</v>
       </c>
       <c r="P11" s="3">
-        <f>P8-P9-P10</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="Q11" s="3">
-        <f>Q8-Q9-Q10</f>
+        <f t="shared" si="0"/>
         <v>487</v>
       </c>
       <c r="R11" s="3">
-        <f>R8-R9-R10</f>
+        <f t="shared" si="0"/>
         <v>547</v>
       </c>
       <c r="S11" s="3">
-        <f>S8-S9-S10</f>
+        <f t="shared" si="0"/>
         <v>607</v>
       </c>
       <c r="T11" s="3">
-        <f>T8-T9-T10</f>
+        <f t="shared" si="0"/>
         <v>595</v>
       </c>
       <c r="U11" s="3">
-        <f>U8-U9-U10</f>
+        <f t="shared" si="0"/>
         <v>621</v>
       </c>
       <c r="V11" s="3">
-        <f>V8-V9-V10</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>646</v>
       </c>
     </row>
     <row r="12" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -1475,7 +1499,9 @@
       <c r="U12" s="13">
         <v>620</v>
       </c>
-      <c r="V12" s="13"/>
+      <c r="V12" s="13">
+        <v>627</v>
+      </c>
     </row>
     <row r="13" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
@@ -1517,7 +1543,9 @@
       <c r="U13" s="13">
         <v>105</v>
       </c>
-      <c r="V13" s="13"/>
+      <c r="V13" s="13">
+        <v>108</v>
+      </c>
     </row>
     <row r="14" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
@@ -1559,7 +1587,9 @@
       <c r="U14" s="13">
         <v>263</v>
       </c>
-      <c r="V14" s="13"/>
+      <c r="V14" s="13">
+        <v>263</v>
+      </c>
     </row>
     <row r="15" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
@@ -1601,7 +1631,9 @@
       <c r="U15" s="13">
         <v>6</v>
       </c>
-      <c r="V15" s="13"/>
+      <c r="V15" s="13">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
@@ -1643,7 +1675,9 @@
       <c r="U16" s="13">
         <v>32</v>
       </c>
-      <c r="V16" s="13"/>
+      <c r="V16" s="13">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1655,9 +1689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y10" sqref="Y10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1831,7 +1865,7 @@
       </c>
       <c r="V2" s="7">
         <f>District!V2</f>
-        <v>0</v>
+        <v>971</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
@@ -1886,7 +1920,9 @@
       <c r="U3" s="5">
         <v>131</v>
       </c>
-      <c r="V3" s="5"/>
+      <c r="V3" s="5">
+        <v>133</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -1940,7 +1976,9 @@
       <c r="U4" s="5">
         <v>155</v>
       </c>
-      <c r="V4" s="5"/>
+      <c r="V4" s="5">
+        <v>156</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
@@ -1994,7 +2032,9 @@
       <c r="U5" s="5">
         <v>66</v>
       </c>
-      <c r="V5" s="5"/>
+      <c r="V5" s="5">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
@@ -2048,7 +2088,9 @@
       <c r="U6" s="5">
         <v>71</v>
       </c>
-      <c r="V6" s="5"/>
+      <c r="V6" s="5">
+        <v>75</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
@@ -2102,7 +2144,9 @@
       <c r="U7" s="5">
         <v>264</v>
       </c>
-      <c r="V7" s="5"/>
+      <c r="V7" s="5">
+        <v>265</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
@@ -2156,7 +2200,9 @@
       <c r="U8" s="5">
         <v>109</v>
       </c>
-      <c r="V8" s="5"/>
+      <c r="V8" s="5">
+        <v>115</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
@@ -2210,7 +2256,9 @@
       <c r="U9" s="5">
         <v>66</v>
       </c>
-      <c r="V9" s="5"/>
+      <c r="V9" s="5">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
@@ -2264,7 +2312,9 @@
       <c r="U10" s="5">
         <v>92</v>
       </c>
-      <c r="V10" s="5"/>
+      <c r="V10" s="5">
+        <v>93</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
@@ -2352,7 +2402,7 @@
       </c>
       <c r="V11" s="7">
         <f>District!V3</f>
-        <v>0</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
@@ -2407,7 +2457,9 @@
       <c r="U12" s="5">
         <v>36</v>
       </c>
-      <c r="V12" s="5"/>
+      <c r="V12" s="5">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -2461,7 +2513,9 @@
       <c r="U13" s="5">
         <v>31</v>
       </c>
-      <c r="V13" s="5"/>
+      <c r="V13" s="5">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
@@ -2515,7 +2569,9 @@
       <c r="U14" s="5">
         <v>73</v>
       </c>
-      <c r="V14" s="5"/>
+      <c r="V14" s="5">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
@@ -2569,7 +2625,9 @@
       <c r="U15" s="5">
         <v>94</v>
       </c>
-      <c r="V15" s="5"/>
+      <c r="V15" s="5">
+        <v>94</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -2623,7 +2681,9 @@
       <c r="U16" s="5">
         <v>81</v>
       </c>
-      <c r="V16" s="5"/>
+      <c r="V16" s="5">
+        <v>83</v>
+      </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
@@ -2677,7 +2737,9 @@
       <c r="U17" s="5">
         <v>10</v>
       </c>
-      <c r="V17" s="5"/>
+      <c r="V17" s="5">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
@@ -2731,7 +2793,9 @@
       <c r="U18" s="5">
         <v>35</v>
       </c>
-      <c r="V18" s="5"/>
+      <c r="V18" s="5">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
@@ -2819,7 +2883,7 @@
       </c>
       <c r="V19" s="7">
         <f>District!V4</f>
-        <v>0</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.35">
@@ -2874,7 +2938,9 @@
       <c r="U20" s="5">
         <v>32</v>
       </c>
-      <c r="V20" s="5"/>
+      <c r="V20" s="5">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
@@ -2928,7 +2994,9 @@
       <c r="U21" s="5">
         <v>4</v>
       </c>
-      <c r="V21" s="5"/>
+      <c r="V21" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -2982,7 +3050,9 @@
       <c r="U22" s="5">
         <v>59</v>
       </c>
-      <c r="V22" s="5"/>
+      <c r="V22" s="5">
+        <v>67</v>
+      </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
@@ -3036,7 +3106,9 @@
       <c r="U23" s="5">
         <v>55</v>
       </c>
-      <c r="V23" s="5"/>
+      <c r="V23" s="5">
+        <v>56</v>
+      </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
@@ -3090,7 +3162,9 @@
       <c r="U24" s="5">
         <v>3</v>
       </c>
-      <c r="V24" s="5"/>
+      <c r="V24" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
@@ -3144,7 +3218,9 @@
       <c r="U25" s="5">
         <v>47</v>
       </c>
-      <c r="V25" s="5"/>
+      <c r="V25" s="5">
+        <v>49</v>
+      </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
@@ -3198,7 +3274,9 @@
       <c r="U26" s="5">
         <v>5</v>
       </c>
-      <c r="V26" s="5"/>
+      <c r="V26" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
@@ -3252,7 +3330,9 @@
       <c r="U27" s="5">
         <v>6</v>
       </c>
-      <c r="V27" s="5"/>
+      <c r="V27" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
@@ -3340,7 +3420,7 @@
       </c>
       <c r="V28" s="7">
         <f>District!V5</f>
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.35">
@@ -3395,7 +3475,9 @@
       <c r="U29" s="5">
         <v>3</v>
       </c>
-      <c r="V29" s="5"/>
+      <c r="V29" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
@@ -3449,7 +3531,9 @@
       <c r="U30" s="5">
         <v>14</v>
       </c>
-      <c r="V30" s="5"/>
+      <c r="V30" s="5">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
@@ -3503,7 +3587,9 @@
       <c r="U31" s="5">
         <v>4</v>
       </c>
-      <c r="V31" s="5"/>
+      <c r="V31" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
@@ -3557,7 +3643,9 @@
       <c r="U32" s="5">
         <v>0</v>
       </c>
-      <c r="V32" s="5"/>
+      <c r="V32" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
@@ -3645,7 +3733,7 @@
       </c>
       <c r="V33" s="7">
         <f>District!V6</f>
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.35">
@@ -3700,7 +3788,9 @@
       <c r="U34" s="5">
         <v>36</v>
       </c>
-      <c r="V34" s="5"/>
+      <c r="V34" s="5">
+        <v>36</v>
+      </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
@@ -3754,7 +3844,9 @@
       <c r="U35" s="5">
         <v>10</v>
       </c>
-      <c r="V35" s="5"/>
+      <c r="V35" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
@@ -3808,7 +3900,9 @@
       <c r="U36" s="5">
         <v>3</v>
       </c>
-      <c r="V36" s="5"/>
+      <c r="V36" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
@@ -3862,7 +3956,9 @@
       <c r="U37" s="10">
         <v>2</v>
       </c>
-      <c r="V37" s="10"/>
+      <c r="V37" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
@@ -3950,7 +4046,7 @@
       </c>
       <c r="V38" s="11">
         <f>District!V7</f>
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -4039,7 +4135,7 @@
       </c>
       <c r="V39" s="11">
         <f>District!V8</f>
-        <v>0</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="40" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -4128,7 +4224,7 @@
       </c>
       <c r="V40" s="11">
         <f>District!V9</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -4217,7 +4313,7 @@
       </c>
       <c r="V41" s="11">
         <f>District!V10</f>
-        <v>0</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="42" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -4306,7 +4402,7 @@
       </c>
       <c r="V42" s="11">
         <f>District!V11</f>
-        <v>0</v>
+        <v>646</v>
       </c>
     </row>
     <row r="43" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -4364,6 +4460,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C44669B21B127D45AF6F62C9A293CCC7" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a3b65afc6cbe717343e4256a9fdd90e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="04f85633-9dbd-493d-9c0a-002b900dde1c" xmlns:ns4="1f157ad2-2ae5-4763-9ea7-a4403f644984" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="de83bd4fc27362efc22842edd0fa359c" ns3:_="" ns4:_="">
     <xsd:import namespace="04f85633-9dbd-493d-9c0a-002b900dde1c"/>
@@ -4580,12 +4682,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F13BE49F-5AB0-4CF9-A4E6-9B8400ED2BB7}">
   <ds:schemaRefs>
@@ -4595,6 +4691,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51454EB7-2533-4710-B1B7-84600D145D91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B495C0-610E-423A-AAC4-17117BBB3EAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4611,13 +4716,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51454EB7-2533-4710-B1B7-84600D145D91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>